<commit_message>
Update basaltic glass analysis - major, wd scans and D2872
</commit_message>
<xml_diff>
--- a/data/processed/basaltic_glasses/calczaf_files/D2872/calczaf_outputs.xlsx
+++ b/data/processed/basaltic_glasses/calczaf_files/D2872/calczaf_outputs.xlsx
@@ -3989,58 +3989,58 @@
         <v>13</v>
       </c>
       <c r="B10">
+        <v>0.575</v>
+      </c>
+      <c r="C10">
+        <v>0.573</v>
+      </c>
+      <c r="D10">
+        <v>0.577</v>
+      </c>
+      <c r="E10">
+        <v>0.583</v>
+      </c>
+      <c r="F10">
         <v>0.576</v>
       </c>
-      <c r="C10">
-        <v>0.575</v>
-      </c>
-      <c r="D10">
+      <c r="G10">
+        <v>0.581</v>
+      </c>
+      <c r="H10">
+        <v>0.582</v>
+      </c>
+      <c r="I10">
         <v>0.578</v>
       </c>
-      <c r="E10">
-        <v>0.585</v>
-      </c>
-      <c r="F10">
+      <c r="J10">
+        <v>0.58</v>
+      </c>
+      <c r="K10">
+        <v>0.579</v>
+      </c>
+      <c r="L10">
         <v>0.577</v>
       </c>
-      <c r="G10">
+      <c r="M10">
         <v>0.582</v>
       </c>
-      <c r="H10">
-        <v>0.583</v>
-      </c>
-      <c r="I10">
-        <v>0.58</v>
-      </c>
-      <c r="J10">
-        <v>0.581</v>
-      </c>
-      <c r="K10">
-        <v>0.58</v>
-      </c>
-      <c r="L10">
-        <v>0.579</v>
-      </c>
-      <c r="M10">
-        <v>0.584</v>
-      </c>
       <c r="N10">
-        <v>0.58</v>
+        <v>0.577</v>
       </c>
       <c r="O10">
-        <v>0.579</v>
+        <v>0.577</v>
       </c>
       <c r="P10">
-        <v>0.58</v>
+        <v>0.578</v>
       </c>
       <c r="Q10">
         <v>0.003</v>
       </c>
       <c r="R10">
-        <v>0.575</v>
+        <v>0.573</v>
       </c>
       <c r="S10">
-        <v>0.585</v>
+        <v>0.583</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -4048,58 +4048,58 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.201</v>
+        <v>0.215</v>
       </c>
       <c r="C11">
-        <v>0.211</v>
+        <v>0.227</v>
       </c>
       <c r="D11">
-        <v>0.181</v>
+        <v>0.193</v>
       </c>
       <c r="E11">
-        <v>0.126</v>
+        <v>0.141</v>
       </c>
       <c r="F11">
-        <v>0.19</v>
+        <v>0.204</v>
       </c>
       <c r="G11">
-        <v>0.15</v>
+        <v>0.162</v>
       </c>
       <c r="H11">
-        <v>0.142</v>
+        <v>0.153</v>
       </c>
       <c r="I11">
-        <v>0.171</v>
+        <v>0.185</v>
       </c>
       <c r="J11">
-        <v>0.155</v>
+        <v>0.165</v>
       </c>
       <c r="K11">
-        <v>0.167</v>
+        <v>0.175</v>
       </c>
       <c r="L11">
-        <v>0.179</v>
+        <v>0.194</v>
       </c>
       <c r="M11">
-        <v>0.135</v>
+        <v>0.148</v>
       </c>
       <c r="N11">
-        <v>0.17</v>
+        <v>0.192</v>
       </c>
       <c r="O11">
-        <v>0.173</v>
+        <v>0.192</v>
       </c>
       <c r="P11">
-        <v>0.168</v>
+        <v>0.182</v>
       </c>
       <c r="Q11">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="R11">
-        <v>0.126</v>
+        <v>0.141</v>
       </c>
       <c r="S11">
-        <v>0.211</v>
+        <v>0.227</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -4343,58 +4343,58 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>46.211</v>
+        <v>46.199</v>
       </c>
       <c r="C16">
-        <v>46.202</v>
+        <v>46.188</v>
       </c>
       <c r="D16">
-        <v>46.229</v>
+        <v>46.218</v>
       </c>
       <c r="E16">
-        <v>46.277</v>
+        <v>46.264</v>
       </c>
       <c r="F16">
-        <v>46.22</v>
+        <v>46.208</v>
       </c>
       <c r="G16">
-        <v>46.256</v>
+        <v>46.246</v>
       </c>
       <c r="H16">
-        <v>46.263</v>
+        <v>46.253</v>
       </c>
       <c r="I16">
-        <v>46.237</v>
+        <v>46.225</v>
       </c>
       <c r="J16">
-        <v>46.252</v>
+        <v>46.243</v>
       </c>
       <c r="K16">
-        <v>46.241</v>
+        <v>46.234</v>
       </c>
       <c r="L16">
-        <v>46.23</v>
+        <v>46.217</v>
       </c>
       <c r="M16">
-        <v>46.269</v>
+        <v>46.258</v>
       </c>
       <c r="N16">
-        <v>46.238</v>
+        <v>46.219</v>
       </c>
       <c r="O16">
-        <v>46.236</v>
+        <v>46.219</v>
       </c>
       <c r="P16">
-        <v>46.24</v>
+        <v>46.228</v>
       </c>
       <c r="Q16">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
       <c r="R16">
-        <v>46.202</v>
+        <v>46.188</v>
       </c>
       <c r="S16">
-        <v>46.277</v>
+        <v>46.264</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -4992,58 +4992,58 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>5.15</v>
+        <v>5.136</v>
       </c>
       <c r="C28">
-        <v>5.14</v>
+        <v>5.124</v>
       </c>
       <c r="D28">
-        <v>5.17</v>
+        <v>5.157</v>
       </c>
       <c r="E28">
-        <v>5.224</v>
+        <v>5.209</v>
       </c>
       <c r="F28">
-        <v>5.16</v>
+        <v>5.147</v>
       </c>
       <c r="G28">
-        <v>5.2</v>
+        <v>5.189</v>
       </c>
       <c r="H28">
-        <v>5.208</v>
+        <v>5.197</v>
       </c>
       <c r="I28">
-        <v>5.18</v>
+        <v>5.165</v>
       </c>
       <c r="J28">
-        <v>5.196</v>
+        <v>5.186</v>
       </c>
       <c r="K28">
-        <v>5.183</v>
+        <v>5.176</v>
       </c>
       <c r="L28">
-        <v>5.171</v>
+        <v>5.156</v>
       </c>
       <c r="M28">
-        <v>5.216</v>
+        <v>5.203</v>
       </c>
       <c r="N28">
-        <v>5.18</v>
+        <v>5.159</v>
       </c>
       <c r="O28">
-        <v>5.178</v>
+        <v>5.159</v>
       </c>
       <c r="P28">
-        <v>5.183</v>
+        <v>5.169</v>
       </c>
       <c r="Q28">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="R28">
-        <v>5.14</v>
+        <v>5.124</v>
       </c>
       <c r="S28">
-        <v>5.224</v>
+        <v>5.209</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -5051,58 +5051,58 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>0.201</v>
+        <v>0.215</v>
       </c>
       <c r="C29">
-        <v>0.211</v>
+        <v>0.227</v>
       </c>
       <c r="D29">
-        <v>0.181</v>
+        <v>0.193</v>
       </c>
       <c r="E29">
-        <v>0.126</v>
+        <v>0.141</v>
       </c>
       <c r="F29">
-        <v>0.19</v>
+        <v>0.204</v>
       </c>
       <c r="G29">
-        <v>0.15</v>
+        <v>0.162</v>
       </c>
       <c r="H29">
-        <v>0.142</v>
+        <v>0.153</v>
       </c>
       <c r="I29">
-        <v>0.171</v>
+        <v>0.185</v>
       </c>
       <c r="J29">
-        <v>0.155</v>
+        <v>0.165</v>
       </c>
       <c r="K29">
-        <v>0.167</v>
+        <v>0.175</v>
       </c>
       <c r="L29">
-        <v>0.179</v>
+        <v>0.194</v>
       </c>
       <c r="M29">
-        <v>0.135</v>
+        <v>0.148</v>
       </c>
       <c r="N29">
-        <v>0.17</v>
+        <v>0.192</v>
       </c>
       <c r="O29">
-        <v>0.173</v>
+        <v>0.192</v>
       </c>
       <c r="P29">
-        <v>0.168</v>
+        <v>0.182</v>
       </c>
       <c r="Q29">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="R29">
-        <v>0.126</v>
+        <v>0.141</v>
       </c>
       <c r="S29">
-        <v>0.211</v>
+        <v>0.227</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -5464,58 +5464,58 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>15.459</v>
+        <v>15.463</v>
       </c>
       <c r="C37">
-        <v>15.461</v>
+        <v>15.466</v>
       </c>
       <c r="D37">
+        <v>15.457</v>
+      </c>
+      <c r="E37">
+        <v>15.442</v>
+      </c>
+      <c r="F37">
+        <v>15.46</v>
+      </c>
+      <c r="G37">
+        <v>15.448</v>
+      </c>
+      <c r="H37">
+        <v>15.445</v>
+      </c>
+      <c r="I37">
+        <v>15.454</v>
+      </c>
+      <c r="J37">
+        <v>15.449</v>
+      </c>
+      <c r="K37">
+        <v>15.451</v>
+      </c>
+      <c r="L37">
+        <v>15.457</v>
+      </c>
+      <c r="M37">
+        <v>15.444</v>
+      </c>
+      <c r="N37">
+        <v>15.456</v>
+      </c>
+      <c r="O37">
+        <v>15.456</v>
+      </c>
+      <c r="P37">
         <v>15.453</v>
-      </c>
-      <c r="E37">
-        <v>15.438</v>
-      </c>
-      <c r="F37">
-        <v>15.456</v>
-      </c>
-      <c r="G37">
-        <v>15.445</v>
-      </c>
-      <c r="H37">
-        <v>15.442</v>
-      </c>
-      <c r="I37">
-        <v>15.45</v>
-      </c>
-      <c r="J37">
-        <v>15.446</v>
-      </c>
-      <c r="K37">
-        <v>15.449</v>
-      </c>
-      <c r="L37">
-        <v>15.453</v>
-      </c>
-      <c r="M37">
-        <v>15.44</v>
-      </c>
-      <c r="N37">
-        <v>15.45</v>
-      </c>
-      <c r="O37">
-        <v>15.451</v>
-      </c>
-      <c r="P37">
-        <v>15.45</v>
       </c>
       <c r="Q37">
         <v>0.007</v>
       </c>
       <c r="R37">
-        <v>15.438</v>
+        <v>15.442</v>
       </c>
       <c r="S37">
-        <v>15.461</v>
+        <v>15.466</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -5523,58 +5523,58 @@
         <v>6</v>
       </c>
       <c r="B38">
+        <v>5.732</v>
+      </c>
+      <c r="C38">
+        <v>5.733</v>
+      </c>
+      <c r="D38">
+        <v>5.73</v>
+      </c>
+      <c r="E38">
+        <v>5.725</v>
+      </c>
+      <c r="F38">
         <v>5.731</v>
       </c>
-      <c r="C38">
-        <v>5.732</v>
-      </c>
-      <c r="D38">
+      <c r="G38">
+        <v>5.727</v>
+      </c>
+      <c r="H38">
+        <v>5.726</v>
+      </c>
+      <c r="I38">
         <v>5.729</v>
       </c>
-      <c r="E38">
-        <v>5.723</v>
-      </c>
-      <c r="F38">
+      <c r="J38">
+        <v>5.727</v>
+      </c>
+      <c r="K38">
+        <v>5.728</v>
+      </c>
+      <c r="L38">
         <v>5.73</v>
       </c>
-      <c r="G38">
-        <v>5.726</v>
-      </c>
-      <c r="H38">
+      <c r="M38">
         <v>5.725</v>
       </c>
-      <c r="I38">
-        <v>5.728</v>
-      </c>
-      <c r="J38">
-        <v>5.726</v>
-      </c>
-      <c r="K38">
-        <v>5.727</v>
-      </c>
-      <c r="L38">
-        <v>5.728</v>
-      </c>
-      <c r="M38">
-        <v>5.724</v>
-      </c>
       <c r="N38">
-        <v>5.728</v>
+        <v>5.73</v>
       </c>
       <c r="O38">
-        <v>5.728</v>
+        <v>5.73</v>
       </c>
       <c r="P38">
-        <v>5.727</v>
+        <v>5.729</v>
       </c>
       <c r="Q38">
         <v>0.003</v>
       </c>
       <c r="R38">
-        <v>5.723</v>
+        <v>5.725</v>
       </c>
       <c r="S38">
-        <v>5.732</v>
+        <v>5.733</v>
       </c>
     </row>
     <row r="39" spans="1:19">
@@ -5582,58 +5582,58 @@
         <v>7</v>
       </c>
       <c r="B39">
+        <v>4.963</v>
+      </c>
+      <c r="C39">
+        <v>4.964</v>
+      </c>
+      <c r="D39">
+        <v>4.961</v>
+      </c>
+      <c r="E39">
+        <v>4.957</v>
+      </c>
+      <c r="F39">
         <v>4.962</v>
-      </c>
-      <c r="C39">
-        <v>4.963</v>
-      </c>
-      <c r="D39">
-        <v>4.96</v>
-      </c>
-      <c r="E39">
-        <v>4.955</v>
-      </c>
-      <c r="F39">
-        <v>4.961</v>
       </c>
       <c r="G39">
         <v>4.958</v>
       </c>
       <c r="H39">
+        <v>4.958</v>
+      </c>
+      <c r="I39">
+        <v>4.961</v>
+      </c>
+      <c r="J39">
+        <v>4.959</v>
+      </c>
+      <c r="K39">
+        <v>4.96</v>
+      </c>
+      <c r="L39">
+        <v>4.961</v>
+      </c>
+      <c r="M39">
         <v>4.957</v>
       </c>
-      <c r="I39">
-        <v>4.959</v>
-      </c>
-      <c r="J39">
-        <v>4.958</v>
-      </c>
-      <c r="K39">
-        <v>4.959</v>
-      </c>
-      <c r="L39">
+      <c r="N39">
+        <v>4.961</v>
+      </c>
+      <c r="O39">
+        <v>4.961</v>
+      </c>
+      <c r="P39">
         <v>4.96</v>
-      </c>
-      <c r="M39">
-        <v>4.956</v>
-      </c>
-      <c r="N39">
-        <v>4.959</v>
-      </c>
-      <c r="O39">
-        <v>4.96</v>
-      </c>
-      <c r="P39">
-        <v>4.959</v>
       </c>
       <c r="Q39">
         <v>0.002</v>
       </c>
       <c r="R39">
-        <v>4.955</v>
+        <v>4.957</v>
       </c>
       <c r="S39">
-        <v>4.963</v>
+        <v>4.964</v>
       </c>
     </row>
     <row r="40" spans="1:19">
@@ -5641,28 +5641,28 @@
         <v>8</v>
       </c>
       <c r="B40">
+        <v>4.148</v>
+      </c>
+      <c r="C40">
+        <v>4.149</v>
+      </c>
+      <c r="D40">
         <v>4.147</v>
       </c>
-      <c r="C40">
-        <v>4.148</v>
-      </c>
-      <c r="D40">
+      <c r="E40">
+        <v>4.143</v>
+      </c>
+      <c r="F40">
+        <v>4.147</v>
+      </c>
+      <c r="G40">
+        <v>4.144</v>
+      </c>
+      <c r="H40">
+        <v>4.144</v>
+      </c>
+      <c r="I40">
         <v>4.146</v>
-      </c>
-      <c r="E40">
-        <v>4.142</v>
-      </c>
-      <c r="F40">
-        <v>4.146</v>
-      </c>
-      <c r="G40">
-        <v>4.143</v>
-      </c>
-      <c r="H40">
-        <v>4.143</v>
-      </c>
-      <c r="I40">
-        <v>4.145</v>
       </c>
       <c r="J40">
         <v>4.144</v>
@@ -5671,28 +5671,28 @@
         <v>4.145</v>
       </c>
       <c r="L40">
+        <v>4.147</v>
+      </c>
+      <c r="M40">
+        <v>4.143</v>
+      </c>
+      <c r="N40">
+        <v>4.147</v>
+      </c>
+      <c r="O40">
+        <v>4.147</v>
+      </c>
+      <c r="P40">
         <v>4.146</v>
-      </c>
-      <c r="M40">
-        <v>4.142</v>
-      </c>
-      <c r="N40">
-        <v>4.145</v>
-      </c>
-      <c r="O40">
-        <v>4.145</v>
-      </c>
-      <c r="P40">
-        <v>4.145</v>
       </c>
       <c r="Q40">
         <v>0.002</v>
       </c>
       <c r="R40">
-        <v>4.142</v>
+        <v>4.143</v>
       </c>
       <c r="S40">
-        <v>4.148</v>
+        <v>4.149</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -5877,7 +5877,7 @@
         <v>12</v>
       </c>
       <c r="B44">
-        <v>1.057</v>
+        <v>1.058</v>
       </c>
       <c r="C44">
         <v>1.058</v>
@@ -5892,7 +5892,7 @@
         <v>1.057</v>
       </c>
       <c r="G44">
-        <v>1.056</v>
+        <v>1.057</v>
       </c>
       <c r="H44">
         <v>1.056</v>
@@ -5936,58 +5936,58 @@
         <v>13</v>
       </c>
       <c r="B45">
-        <v>10.866</v>
+        <v>10.84</v>
       </c>
       <c r="C45">
-        <v>10.848</v>
+        <v>10.816</v>
       </c>
       <c r="D45">
-        <v>10.904</v>
+        <v>10.88</v>
       </c>
       <c r="E45">
-        <v>11.009</v>
+        <v>10.98</v>
       </c>
       <c r="F45">
-        <v>10.887</v>
+        <v>10.861</v>
       </c>
       <c r="G45">
-        <v>10.963</v>
+        <v>10.941</v>
       </c>
       <c r="H45">
-        <v>10.978</v>
+        <v>10.957</v>
       </c>
       <c r="I45">
-        <v>10.923</v>
+        <v>10.896</v>
       </c>
       <c r="J45">
-        <v>10.954</v>
+        <v>10.935</v>
       </c>
       <c r="K45">
-        <v>10.93</v>
+        <v>10.916</v>
       </c>
       <c r="L45">
-        <v>10.908</v>
+        <v>10.879</v>
       </c>
       <c r="M45">
-        <v>10.992</v>
+        <v>10.968</v>
       </c>
       <c r="N45">
-        <v>10.924</v>
+        <v>10.884</v>
       </c>
       <c r="O45">
-        <v>10.92</v>
+        <v>10.883</v>
       </c>
       <c r="P45">
-        <v>10.929</v>
+        <v>10.903</v>
       </c>
       <c r="Q45">
-        <v>0.046</v>
+        <v>0.049</v>
       </c>
       <c r="R45">
-        <v>10.848</v>
+        <v>10.816</v>
       </c>
       <c r="S45">
-        <v>11.009</v>
+        <v>10.98</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -5995,58 +5995,58 @@
         <v>14</v>
       </c>
       <c r="B46">
-        <v>0.272</v>
+        <v>0.291</v>
       </c>
       <c r="C46">
-        <v>0.286</v>
+        <v>0.308</v>
       </c>
       <c r="D46">
-        <v>0.245</v>
+        <v>0.262</v>
       </c>
       <c r="E46">
-        <v>0.171</v>
+        <v>0.192</v>
       </c>
       <c r="F46">
-        <v>0.258</v>
+        <v>0.276</v>
       </c>
       <c r="G46">
-        <v>0.204</v>
+        <v>0.219</v>
       </c>
       <c r="H46">
-        <v>0.193</v>
+        <v>0.208</v>
       </c>
       <c r="I46">
-        <v>0.232</v>
+        <v>0.251</v>
       </c>
       <c r="J46">
-        <v>0.21</v>
+        <v>0.223</v>
       </c>
       <c r="K46">
-        <v>0.227</v>
+        <v>0.237</v>
       </c>
       <c r="L46">
-        <v>0.243</v>
+        <v>0.264</v>
       </c>
       <c r="M46">
-        <v>0.183</v>
+        <v>0.2</v>
       </c>
       <c r="N46">
-        <v>0.231</v>
+        <v>0.26</v>
       </c>
       <c r="O46">
-        <v>0.234</v>
+        <v>0.26</v>
       </c>
       <c r="P46">
-        <v>0.228</v>
+        <v>0.247</v>
       </c>
       <c r="Q46">
-        <v>0.033</v>
+        <v>0.035</v>
       </c>
       <c r="R46">
-        <v>0.171</v>
+        <v>0.192</v>
       </c>
       <c r="S46">
-        <v>0.286</v>
+        <v>0.308</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -6116,46 +6116,46 @@
         <v>2.356</v>
       </c>
       <c r="C48">
+        <v>2.357</v>
+      </c>
+      <c r="D48">
         <v>2.356</v>
-      </c>
-      <c r="D48">
-        <v>2.355</v>
       </c>
       <c r="E48">
         <v>2.353</v>
       </c>
       <c r="F48">
-        <v>2.355</v>
+        <v>2.356</v>
       </c>
       <c r="G48">
         <v>2.354</v>
       </c>
       <c r="H48">
-        <v>2.353</v>
+        <v>2.354</v>
       </c>
       <c r="I48">
-        <v>2.354</v>
+        <v>2.355</v>
       </c>
       <c r="J48">
         <v>2.354</v>
       </c>
       <c r="K48">
+        <v>2.355</v>
+      </c>
+      <c r="L48">
+        <v>2.356</v>
+      </c>
+      <c r="M48">
         <v>2.354</v>
       </c>
-      <c r="L48">
+      <c r="N48">
         <v>2.355</v>
-      </c>
-      <c r="M48">
-        <v>2.353</v>
-      </c>
-      <c r="N48">
-        <v>2.354</v>
       </c>
       <c r="O48">
         <v>2.355</v>
       </c>
       <c r="P48">
-        <v>2.354</v>
+        <v>2.355</v>
       </c>
       <c r="Q48">
         <v>0.001</v>
@@ -6164,7 +6164,7 @@
         <v>2.353</v>
       </c>
       <c r="S48">
-        <v>2.356</v>
+        <v>2.357</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -6290,58 +6290,58 @@
         <v>19</v>
       </c>
       <c r="B51">
+        <v>54.897</v>
+      </c>
+      <c r="C51">
+        <v>54.896</v>
+      </c>
+      <c r="D51">
         <v>54.898</v>
       </c>
-      <c r="C51">
+      <c r="E51">
+        <v>54.901</v>
+      </c>
+      <c r="F51">
         <v>54.897</v>
       </c>
-      <c r="D51">
-        <v>54.899</v>
-      </c>
-      <c r="E51">
-        <v>54.902</v>
-      </c>
-      <c r="F51">
+      <c r="G51">
+        <v>54.9</v>
+      </c>
+      <c r="H51">
+        <v>54.9</v>
+      </c>
+      <c r="I51">
         <v>54.898</v>
-      </c>
-      <c r="G51">
-        <v>54.901</v>
-      </c>
-      <c r="H51">
-        <v>54.901</v>
-      </c>
-      <c r="I51">
-        <v>54.899</v>
       </c>
       <c r="J51">
         <v>54.9</v>
       </c>
       <c r="K51">
-        <v>54.9</v>
+        <v>54.899</v>
       </c>
       <c r="L51">
+        <v>54.898</v>
+      </c>
+      <c r="M51">
+        <v>54.901</v>
+      </c>
+      <c r="N51">
+        <v>54.898</v>
+      </c>
+      <c r="O51">
+        <v>54.898</v>
+      </c>
+      <c r="P51">
         <v>54.899</v>
-      </c>
-      <c r="M51">
-        <v>54.902</v>
-      </c>
-      <c r="N51">
-        <v>54.899</v>
-      </c>
-      <c r="O51">
-        <v>54.899</v>
-      </c>
-      <c r="P51">
-        <v>54.9</v>
       </c>
       <c r="Q51">
         <v>0.002</v>
       </c>
       <c r="R51">
-        <v>54.897</v>
+        <v>54.896</v>
       </c>
       <c r="S51">
-        <v>54.902</v>
+        <v>54.901</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -6955,58 +6955,58 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.572</v>
+        <v>0.57</v>
       </c>
       <c r="C10">
-        <v>0.57</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="D10">
+        <v>0.573</v>
+      </c>
+      <c r="E10">
+        <v>0.58</v>
+      </c>
+      <c r="F10">
+        <v>0.571</v>
+      </c>
+      <c r="G10">
+        <v>0.577</v>
+      </c>
+      <c r="H10">
+        <v>0.578</v>
+      </c>
+      <c r="I10">
         <v>0.574</v>
       </c>
-      <c r="E10">
-        <v>0.582</v>
-      </c>
-      <c r="F10">
+      <c r="J10">
+        <v>0.577</v>
+      </c>
+      <c r="K10">
+        <v>0.575</v>
+      </c>
+      <c r="L10">
         <v>0.573</v>
       </c>
-      <c r="G10">
-        <v>0.578</v>
-      </c>
-      <c r="H10">
-        <v>0.58</v>
-      </c>
-      <c r="I10">
-        <v>0.576</v>
-      </c>
-      <c r="J10">
-        <v>0.578</v>
-      </c>
-      <c r="K10">
-        <v>0.576</v>
-      </c>
-      <c r="L10">
-        <v>0.575</v>
-      </c>
       <c r="M10">
-        <v>0.581</v>
+        <v>0.579</v>
       </c>
       <c r="N10">
-        <v>0.576</v>
+        <v>0.573</v>
       </c>
       <c r="O10">
-        <v>0.575</v>
+        <v>0.573</v>
       </c>
       <c r="P10">
-        <v>0.576</v>
+        <v>0.574</v>
       </c>
       <c r="Q10">
         <v>0.003</v>
       </c>
       <c r="R10">
-        <v>0.57</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="S10">
-        <v>0.582</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -7014,58 +7014,58 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.242</v>
+        <v>0.259</v>
       </c>
       <c r="C11">
-        <v>0.254</v>
+        <v>0.273</v>
       </c>
       <c r="D11">
-        <v>0.218</v>
+        <v>0.233</v>
       </c>
       <c r="E11">
-        <v>0.152</v>
+        <v>0.17</v>
       </c>
       <c r="F11">
-        <v>0.229</v>
+        <v>0.245</v>
       </c>
       <c r="G11">
-        <v>0.181</v>
+        <v>0.195</v>
       </c>
       <c r="H11">
-        <v>0.171</v>
+        <v>0.185</v>
       </c>
       <c r="I11">
-        <v>0.206</v>
+        <v>0.223</v>
       </c>
       <c r="J11">
-        <v>0.187</v>
+        <v>0.198</v>
       </c>
       <c r="K11">
-        <v>0.202</v>
+        <v>0.211</v>
       </c>
       <c r="L11">
-        <v>0.216</v>
+        <v>0.234</v>
       </c>
       <c r="M11">
-        <v>0.163</v>
+        <v>0.178</v>
       </c>
       <c r="N11">
-        <v>0.205</v>
+        <v>0.231</v>
       </c>
       <c r="O11">
-        <v>0.208</v>
+        <v>0.231</v>
       </c>
       <c r="P11">
-        <v>0.202</v>
+        <v>0.219</v>
       </c>
       <c r="Q11">
-        <v>0.029</v>
+        <v>0.031</v>
       </c>
       <c r="R11">
-        <v>0.152</v>
+        <v>0.17</v>
       </c>
       <c r="S11">
-        <v>0.254</v>
+        <v>0.273</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -7309,58 +7309,58 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>46.174</v>
+        <v>46.16</v>
       </c>
       <c r="C16">
-        <v>46.164</v>
+        <v>46.146</v>
       </c>
       <c r="D16">
-        <v>46.196</v>
+        <v>46.182</v>
       </c>
       <c r="E16">
-        <v>46.254</v>
+        <v>46.238</v>
       </c>
       <c r="F16">
-        <v>46.186</v>
+        <v>46.171</v>
       </c>
       <c r="G16">
-        <v>46.228</v>
+        <v>46.216</v>
       </c>
       <c r="H16">
-        <v>46.237</v>
+        <v>46.225</v>
       </c>
       <c r="I16">
-        <v>46.206</v>
+        <v>46.191</v>
       </c>
       <c r="J16">
-        <v>46.223</v>
+        <v>46.213</v>
       </c>
       <c r="K16">
-        <v>46.21</v>
+        <v>46.202</v>
       </c>
       <c r="L16">
-        <v>46.198</v>
+        <v>46.182</v>
       </c>
       <c r="M16">
-        <v>46.245</v>
+        <v>46.231</v>
       </c>
       <c r="N16">
-        <v>46.207</v>
+        <v>46.184</v>
       </c>
       <c r="O16">
-        <v>46.204</v>
+        <v>46.184</v>
       </c>
       <c r="P16">
-        <v>46.21</v>
+        <v>46.195</v>
       </c>
       <c r="Q16">
-        <v>0.026</v>
+        <v>0.027</v>
       </c>
       <c r="R16">
-        <v>46.164</v>
+        <v>46.146</v>
       </c>
       <c r="S16">
-        <v>46.254</v>
+        <v>46.238</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -7958,58 +7958,58 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>5.109</v>
+        <v>5.092</v>
       </c>
       <c r="C28">
-        <v>5.097</v>
+        <v>5.077</v>
       </c>
       <c r="D28">
-        <v>5.133</v>
+        <v>5.118</v>
       </c>
       <c r="E28">
-        <v>5.199</v>
+        <v>5.18</v>
       </c>
       <c r="F28">
-        <v>5.122</v>
+        <v>5.105</v>
       </c>
       <c r="G28">
-        <v>5.169</v>
+        <v>5.156</v>
       </c>
       <c r="H28">
-        <v>5.179</v>
+        <v>5.166</v>
       </c>
       <c r="I28">
-        <v>5.144</v>
+        <v>5.127</v>
       </c>
       <c r="J28">
-        <v>5.164</v>
+        <v>5.152</v>
       </c>
       <c r="K28">
-        <v>5.149</v>
+        <v>5.14</v>
       </c>
       <c r="L28">
-        <v>5.135</v>
+        <v>5.117</v>
       </c>
       <c r="M28">
-        <v>5.188</v>
+        <v>5.173</v>
       </c>
       <c r="N28">
-        <v>5.145</v>
+        <v>5.12</v>
       </c>
       <c r="O28">
-        <v>5.142</v>
+        <v>5.119</v>
       </c>
       <c r="P28">
-        <v>5.148</v>
+        <v>5.132</v>
       </c>
       <c r="Q28">
-        <v>0.029</v>
+        <v>0.031</v>
       </c>
       <c r="R28">
-        <v>5.097</v>
+        <v>5.077</v>
       </c>
       <c r="S28">
-        <v>5.199</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -8017,58 +8017,58 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>0.242</v>
+        <v>0.259</v>
       </c>
       <c r="C29">
-        <v>0.254</v>
+        <v>0.273</v>
       </c>
       <c r="D29">
-        <v>0.218</v>
+        <v>0.233</v>
       </c>
       <c r="E29">
-        <v>0.152</v>
+        <v>0.17</v>
       </c>
       <c r="F29">
-        <v>0.229</v>
+        <v>0.245</v>
       </c>
       <c r="G29">
-        <v>0.181</v>
+        <v>0.195</v>
       </c>
       <c r="H29">
-        <v>0.171</v>
+        <v>0.185</v>
       </c>
       <c r="I29">
-        <v>0.206</v>
+        <v>0.223</v>
       </c>
       <c r="J29">
-        <v>0.187</v>
+        <v>0.198</v>
       </c>
       <c r="K29">
-        <v>0.202</v>
+        <v>0.211</v>
       </c>
       <c r="L29">
-        <v>0.216</v>
+        <v>0.234</v>
       </c>
       <c r="M29">
-        <v>0.163</v>
+        <v>0.178</v>
       </c>
       <c r="N29">
-        <v>0.205</v>
+        <v>0.231</v>
       </c>
       <c r="O29">
-        <v>0.208</v>
+        <v>0.231</v>
       </c>
       <c r="P29">
-        <v>0.202</v>
+        <v>0.219</v>
       </c>
       <c r="Q29">
-        <v>0.029</v>
+        <v>0.031</v>
       </c>
       <c r="R29">
-        <v>0.152</v>
+        <v>0.17</v>
       </c>
       <c r="S29">
-        <v>0.254</v>
+        <v>0.273</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -8430,58 +8430,58 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>15.47</v>
+        <v>15.475</v>
       </c>
       <c r="C37">
-        <v>15.474</v>
+        <v>15.479</v>
       </c>
       <c r="D37">
+        <v>15.468</v>
+      </c>
+      <c r="E37">
+        <v>15.45</v>
+      </c>
+      <c r="F37">
+        <v>15.471</v>
+      </c>
+      <c r="G37">
+        <v>15.457</v>
+      </c>
+      <c r="H37">
+        <v>15.454</v>
+      </c>
+      <c r="I37">
+        <v>15.465</v>
+      </c>
+      <c r="J37">
+        <v>15.458</v>
+      </c>
+      <c r="K37">
+        <v>15.461</v>
+      </c>
+      <c r="L37">
+        <v>15.468</v>
+      </c>
+      <c r="M37">
+        <v>15.452</v>
+      </c>
+      <c r="N37">
+        <v>15.467</v>
+      </c>
+      <c r="O37">
+        <v>15.467</v>
+      </c>
+      <c r="P37">
         <v>15.464</v>
       </c>
-      <c r="E37">
-        <v>15.445</v>
-      </c>
-      <c r="F37">
-        <v>15.467</v>
-      </c>
-      <c r="G37">
-        <v>15.453</v>
-      </c>
-      <c r="H37">
+      <c r="Q37">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="R37">
         <v>15.45</v>
       </c>
-      <c r="I37">
-        <v>15.46</v>
-      </c>
-      <c r="J37">
-        <v>15.455</v>
-      </c>
-      <c r="K37">
-        <v>15.459</v>
-      </c>
-      <c r="L37">
-        <v>15.463</v>
-      </c>
-      <c r="M37">
-        <v>15.448</v>
-      </c>
-      <c r="N37">
-        <v>15.46</v>
-      </c>
-      <c r="O37">
-        <v>15.461</v>
-      </c>
-      <c r="P37">
-        <v>15.459</v>
-      </c>
-      <c r="Q37">
-        <v>0.008</v>
-      </c>
-      <c r="R37">
-        <v>15.445</v>
-      </c>
       <c r="S37">
-        <v>15.474</v>
+        <v>15.479</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -8489,58 +8489,58 @@
         <v>6</v>
       </c>
       <c r="B38">
+        <v>5.737</v>
+      </c>
+      <c r="C38">
+        <v>5.738</v>
+      </c>
+      <c r="D38">
+        <v>5.734</v>
+      </c>
+      <c r="E38">
+        <v>5.728</v>
+      </c>
+      <c r="F38">
         <v>5.735</v>
       </c>
-      <c r="C38">
-        <v>5.736</v>
-      </c>
-      <c r="D38">
+      <c r="G38">
+        <v>5.73</v>
+      </c>
+      <c r="H38">
+        <v>5.729</v>
+      </c>
+      <c r="I38">
+        <v>5.733</v>
+      </c>
+      <c r="J38">
+        <v>5.73</v>
+      </c>
+      <c r="K38">
         <v>5.732</v>
       </c>
-      <c r="E38">
-        <v>5.726</v>
-      </c>
-      <c r="F38">
+      <c r="L38">
         <v>5.734</v>
       </c>
-      <c r="G38">
-        <v>5.729</v>
-      </c>
-      <c r="H38">
+      <c r="M38">
         <v>5.728</v>
       </c>
-      <c r="I38">
-        <v>5.731</v>
-      </c>
-      <c r="J38">
-        <v>5.729</v>
-      </c>
-      <c r="K38">
-        <v>5.731</v>
-      </c>
-      <c r="L38">
-        <v>5.732</v>
-      </c>
-      <c r="M38">
-        <v>5.727</v>
-      </c>
       <c r="N38">
-        <v>5.731</v>
+        <v>5.734</v>
       </c>
       <c r="O38">
-        <v>5.732</v>
+        <v>5.734</v>
       </c>
       <c r="P38">
-        <v>5.731</v>
+        <v>5.733</v>
       </c>
       <c r="Q38">
         <v>0.003</v>
       </c>
       <c r="R38">
-        <v>5.726</v>
+        <v>5.728</v>
       </c>
       <c r="S38">
-        <v>5.736</v>
+        <v>5.738</v>
       </c>
     </row>
     <row r="39" spans="1:19">
@@ -8548,58 +8548,58 @@
         <v>7</v>
       </c>
       <c r="B39">
+        <v>4.967</v>
+      </c>
+      <c r="C39">
+        <v>4.968</v>
+      </c>
+      <c r="D39">
+        <v>4.965</v>
+      </c>
+      <c r="E39">
+        <v>4.959</v>
+      </c>
+      <c r="F39">
         <v>4.966</v>
       </c>
-      <c r="C39">
-        <v>4.967</v>
-      </c>
-      <c r="D39">
+      <c r="G39">
+        <v>4.962</v>
+      </c>
+      <c r="H39">
+        <v>4.961</v>
+      </c>
+      <c r="I39">
         <v>4.964</v>
       </c>
-      <c r="E39">
-        <v>4.958</v>
-      </c>
-      <c r="F39">
+      <c r="J39">
+        <v>4.962</v>
+      </c>
+      <c r="K39">
+        <v>4.963</v>
+      </c>
+      <c r="L39">
+        <v>4.965</v>
+      </c>
+      <c r="M39">
+        <v>4.96</v>
+      </c>
+      <c r="N39">
+        <v>4.965</v>
+      </c>
+      <c r="O39">
+        <v>4.965</v>
+      </c>
+      <c r="P39">
         <v>4.964</v>
-      </c>
-      <c r="G39">
-        <v>4.96</v>
-      </c>
-      <c r="H39">
-        <v>4.959</v>
-      </c>
-      <c r="I39">
-        <v>4.962</v>
-      </c>
-      <c r="J39">
-        <v>4.961</v>
-      </c>
-      <c r="K39">
-        <v>4.962</v>
-      </c>
-      <c r="L39">
-        <v>4.963</v>
-      </c>
-      <c r="M39">
-        <v>4.959</v>
-      </c>
-      <c r="N39">
-        <v>4.962</v>
-      </c>
-      <c r="O39">
-        <v>4.963</v>
-      </c>
-      <c r="P39">
-        <v>4.962</v>
       </c>
       <c r="Q39">
         <v>0.003</v>
       </c>
       <c r="R39">
-        <v>4.958</v>
+        <v>4.959</v>
       </c>
       <c r="S39">
-        <v>4.967</v>
+        <v>4.968</v>
       </c>
     </row>
     <row r="40" spans="1:19">
@@ -8607,58 +8607,58 @@
         <v>8</v>
       </c>
       <c r="B40">
+        <v>4.152</v>
+      </c>
+      <c r="C40">
+        <v>4.153</v>
+      </c>
+      <c r="D40">
         <v>4.15</v>
       </c>
-      <c r="C40">
-        <v>4.151</v>
-      </c>
-      <c r="D40">
+      <c r="E40">
+        <v>4.145</v>
+      </c>
+      <c r="F40">
+        <v>4.15</v>
+      </c>
+      <c r="G40">
+        <v>4.147</v>
+      </c>
+      <c r="H40">
+        <v>4.146</v>
+      </c>
+      <c r="I40">
+        <v>4.149</v>
+      </c>
+      <c r="J40">
+        <v>4.147</v>
+      </c>
+      <c r="K40">
         <v>4.148</v>
       </c>
-      <c r="E40">
-        <v>4.143</v>
-      </c>
-      <c r="F40">
+      <c r="L40">
+        <v>4.15</v>
+      </c>
+      <c r="M40">
+        <v>4.146</v>
+      </c>
+      <c r="N40">
         <v>4.149</v>
       </c>
-      <c r="G40">
-        <v>4.146</v>
-      </c>
-      <c r="H40">
-        <v>4.145</v>
-      </c>
-      <c r="I40">
-        <v>4.148</v>
-      </c>
-      <c r="J40">
-        <v>4.146</v>
-      </c>
-      <c r="K40">
-        <v>4.147</v>
-      </c>
-      <c r="L40">
-        <v>4.148</v>
-      </c>
-      <c r="M40">
-        <v>4.144</v>
-      </c>
-      <c r="N40">
-        <v>4.148</v>
-      </c>
       <c r="O40">
-        <v>4.148</v>
+        <v>4.15</v>
       </c>
       <c r="P40">
-        <v>4.147</v>
+        <v>4.149</v>
       </c>
       <c r="Q40">
         <v>0.002</v>
       </c>
       <c r="R40">
-        <v>4.143</v>
+        <v>4.145</v>
       </c>
       <c r="S40">
-        <v>4.151</v>
+        <v>4.153</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -8843,16 +8843,16 @@
         <v>12</v>
       </c>
       <c r="B44">
-        <v>1.058</v>
+        <v>1.059</v>
       </c>
       <c r="C44">
-        <v>1.058</v>
+        <v>1.059</v>
       </c>
       <c r="D44">
         <v>1.058</v>
       </c>
       <c r="E44">
-        <v>1.056</v>
+        <v>1.057</v>
       </c>
       <c r="F44">
         <v>1.058</v>
@@ -8870,7 +8870,7 @@
         <v>1.057</v>
       </c>
       <c r="K44">
-        <v>1.057</v>
+        <v>1.058</v>
       </c>
       <c r="L44">
         <v>1.058</v>
@@ -8879,22 +8879,22 @@
         <v>1.057</v>
       </c>
       <c r="N44">
-        <v>1.057</v>
+        <v>1.058</v>
       </c>
       <c r="O44">
         <v>1.058</v>
       </c>
       <c r="P44">
-        <v>1.057</v>
+        <v>1.058</v>
       </c>
       <c r="Q44">
         <v>0.001</v>
       </c>
       <c r="R44">
-        <v>1.056</v>
+        <v>1.057</v>
       </c>
       <c r="S44">
-        <v>1.058</v>
+        <v>1.059</v>
       </c>
     </row>
     <row r="45" spans="1:19">
@@ -8902,58 +8902,58 @@
         <v>13</v>
       </c>
       <c r="B45">
-        <v>10.788</v>
+        <v>10.756</v>
       </c>
       <c r="C45">
-        <v>10.765</v>
+        <v>10.727</v>
       </c>
       <c r="D45">
-        <v>10.833</v>
+        <v>10.805</v>
       </c>
       <c r="E45">
-        <v>10.96</v>
+        <v>10.924</v>
       </c>
       <c r="F45">
-        <v>10.812</v>
+        <v>10.781</v>
       </c>
       <c r="G45">
-        <v>10.904</v>
+        <v>10.878</v>
       </c>
       <c r="H45">
-        <v>10.923</v>
+        <v>10.897</v>
       </c>
       <c r="I45">
-        <v>10.856</v>
+        <v>10.823</v>
       </c>
       <c r="J45">
-        <v>10.893</v>
+        <v>10.871</v>
       </c>
       <c r="K45">
-        <v>10.865</v>
+        <v>10.848</v>
       </c>
       <c r="L45">
-        <v>10.838</v>
+        <v>10.803</v>
       </c>
       <c r="M45">
-        <v>10.939</v>
+        <v>10.91</v>
       </c>
       <c r="N45">
-        <v>10.858</v>
+        <v>10.809</v>
       </c>
       <c r="O45">
-        <v>10.852</v>
+        <v>10.808</v>
       </c>
       <c r="P45">
-        <v>10.863</v>
+        <v>10.831</v>
       </c>
       <c r="Q45">
-        <v>0.056</v>
+        <v>0.059</v>
       </c>
       <c r="R45">
-        <v>10.765</v>
+        <v>10.727</v>
       </c>
       <c r="S45">
-        <v>10.96</v>
+        <v>10.924</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -8961,58 +8961,58 @@
         <v>14</v>
       </c>
       <c r="B46">
-        <v>0.328</v>
+        <v>0.351</v>
       </c>
       <c r="C46">
-        <v>0.345</v>
+        <v>0.372</v>
       </c>
       <c r="D46">
-        <v>0.296</v>
+        <v>0.316</v>
       </c>
       <c r="E46">
-        <v>0.206</v>
+        <v>0.231</v>
       </c>
       <c r="F46">
-        <v>0.311</v>
+        <v>0.333</v>
       </c>
       <c r="G46">
-        <v>0.246</v>
+        <v>0.264</v>
       </c>
       <c r="H46">
-        <v>0.232</v>
+        <v>0.25</v>
       </c>
       <c r="I46">
-        <v>0.28</v>
+        <v>0.303</v>
       </c>
       <c r="J46">
-        <v>0.253</v>
+        <v>0.269</v>
       </c>
       <c r="K46">
-        <v>0.274</v>
+        <v>0.286</v>
       </c>
       <c r="L46">
-        <v>0.293</v>
+        <v>0.318</v>
       </c>
       <c r="M46">
-        <v>0.221</v>
+        <v>0.241</v>
       </c>
       <c r="N46">
-        <v>0.279</v>
+        <v>0.313</v>
       </c>
       <c r="O46">
-        <v>0.283</v>
+        <v>0.314</v>
       </c>
       <c r="P46">
-        <v>0.275</v>
+        <v>0.297</v>
       </c>
       <c r="Q46">
-        <v>0.04</v>
+        <v>0.042</v>
       </c>
       <c r="R46">
-        <v>0.206</v>
+        <v>0.231</v>
       </c>
       <c r="S46">
-        <v>0.345</v>
+        <v>0.372</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -9082,46 +9082,46 @@
         <v>2.358</v>
       </c>
       <c r="C48">
-        <v>2.358</v>
+        <v>2.359</v>
       </c>
       <c r="D48">
-        <v>2.356</v>
+        <v>2.357</v>
       </c>
       <c r="E48">
         <v>2.354</v>
       </c>
       <c r="F48">
+        <v>2.358</v>
+      </c>
+      <c r="G48">
+        <v>2.356</v>
+      </c>
+      <c r="H48">
+        <v>2.355</v>
+      </c>
+      <c r="I48">
         <v>2.357</v>
       </c>
-      <c r="G48">
-        <v>2.355</v>
-      </c>
-      <c r="H48">
-        <v>2.354</v>
-      </c>
-      <c r="I48">
+      <c r="J48">
         <v>2.356</v>
-      </c>
-      <c r="J48">
-        <v>2.355</v>
       </c>
       <c r="K48">
         <v>2.356</v>
       </c>
       <c r="L48">
-        <v>2.356</v>
+        <v>2.357</v>
       </c>
       <c r="M48">
-        <v>2.354</v>
+        <v>2.355</v>
       </c>
       <c r="N48">
-        <v>2.356</v>
+        <v>2.357</v>
       </c>
       <c r="O48">
-        <v>2.356</v>
+        <v>2.357</v>
       </c>
       <c r="P48">
-        <v>2.356</v>
+        <v>2.357</v>
       </c>
       <c r="Q48">
         <v>0.001</v>
@@ -9130,7 +9130,7 @@
         <v>2.354</v>
       </c>
       <c r="S48">
-        <v>2.358</v>
+        <v>2.359</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -9256,28 +9256,28 @@
         <v>19</v>
       </c>
       <c r="B51">
-        <v>54.895</v>
+        <v>54.894</v>
       </c>
       <c r="C51">
-        <v>54.894</v>
+        <v>54.893</v>
       </c>
       <c r="D51">
         <v>54.896</v>
       </c>
       <c r="E51">
-        <v>54.9</v>
+        <v>54.899</v>
       </c>
       <c r="F51">
+        <v>54.895</v>
+      </c>
+      <c r="G51">
+        <v>54.898</v>
+      </c>
+      <c r="H51">
+        <v>54.898</v>
+      </c>
+      <c r="I51">
         <v>54.896</v>
-      </c>
-      <c r="G51">
-        <v>54.899</v>
-      </c>
-      <c r="H51">
-        <v>54.899</v>
-      </c>
-      <c r="I51">
-        <v>54.897</v>
       </c>
       <c r="J51">
         <v>54.898</v>
@@ -9286,28 +9286,28 @@
         <v>54.897</v>
       </c>
       <c r="L51">
+        <v>54.895</v>
+      </c>
+      <c r="M51">
+        <v>54.899</v>
+      </c>
+      <c r="N51">
         <v>54.896</v>
       </c>
-      <c r="M51">
-        <v>54.9</v>
-      </c>
-      <c r="N51">
-        <v>54.897</v>
-      </c>
       <c r="O51">
-        <v>54.897</v>
+        <v>54.896</v>
       </c>
       <c r="P51">
-        <v>54.897</v>
+        <v>54.896</v>
       </c>
       <c r="Q51">
         <v>0.002</v>
       </c>
       <c r="R51">
-        <v>54.894</v>
+        <v>54.893</v>
       </c>
       <c r="S51">
-        <v>54.9</v>
+        <v>54.899</v>
       </c>
     </row>
     <row r="52" spans="1:19">

</xml_diff>